<commit_message>
Implementación de Dublin Core en las tablas de metadatos.
</commit_message>
<xml_diff>
--- a/data/metadatos-bga.xlsx
+++ b/data/metadatos-bga.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gemartin/proyectos/coleccion-bga/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE0C792-E7CD-6447-B794-2EC62A939CF5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{6382482E-0D6B-D448-B63C-470E3C6E2DCD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="2320" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{1C8FF9AE-8C38-4140-964F-EDC9CA2419B0}"/>
+    <workbookView xWindow="1020" yWindow="2080" windowWidth="28040" windowHeight="17440" xr2:uid="{1C8FF9AE-8C38-4140-964F-EDC9CA2419B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Obra" sheetId="1" r:id="rId1"/>
@@ -28,21 +28,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>titulo</t>
-  </si>
-  <si>
-    <t>fecha</t>
-  </si>
-  <si>
-    <t>dimensiones</t>
-  </si>
-  <si>
-    <t>tecnica</t>
-  </si>
-  <si>
     <t>archivo</t>
   </si>
   <si>
@@ -58,9 +43,6 @@
     <t>suicidas-sisga-1.jpg</t>
   </si>
   <si>
-    <t>periodico</t>
-  </si>
-  <si>
     <t>Doble suicidio en "El Sisga"</t>
   </si>
   <si>
@@ -122,6 +104,24 @@
   </si>
   <si>
     <t>exmilitar-mata-esposa.jpg</t>
+  </si>
+  <si>
+    <t>dc.title</t>
+  </si>
+  <si>
+    <t>dc.date</t>
+  </si>
+  <si>
+    <t>dc.publisher</t>
+  </si>
+  <si>
+    <t>dc.identifier</t>
+  </si>
+  <si>
+    <t>dc.format</t>
+  </si>
+  <si>
+    <t>dc.medium</t>
   </si>
 </sst>
 </file>
@@ -476,13 +476,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01A9A4AD-6081-8846-938D-44015FD68A87}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.1640625" customWidth="1"/>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
     <col min="2" max="2" width="25.83203125" customWidth="1"/>
     <col min="3" max="3" width="17.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="21.33203125" customWidth="1"/>
@@ -492,22 +492,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -515,19 +515,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -535,19 +535,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -555,19 +555,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -579,13 +579,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDB39985-7B05-6242-99E4-AC6F719B2CB6}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.5" customWidth="1"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="40.33203125" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="20.5" customWidth="1"/>
@@ -594,19 +594,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -614,16 +614,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -631,16 +631,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -648,10 +648,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -659,10 +659,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fechas compatibles con sql, valor NULL en campos vaciós
</commit_message>
<xml_diff>
--- a/data/metadatos-bga.xlsx
+++ b/data/metadatos-bga.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Obra" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -44,7 +44,7 @@
     <t xml:space="preserve">Los Suicidas del Sisga No 1</t>
   </si>
   <si>
-    <t xml:space="preserve">01-01-1965</t>
+    <t xml:space="preserve">1965-01-01</t>
   </si>
   <si>
     <t xml:space="preserve">120x100 cm</t>
@@ -59,7 +59,7 @@
     <t xml:space="preserve">El Paraíso</t>
   </si>
   <si>
-    <t xml:space="preserve">01-01-1997</t>
+    <t xml:space="preserve">1997-01-01</t>
   </si>
   <si>
     <t xml:space="preserve">160x45 cm</t>
@@ -71,7 +71,7 @@
     <t xml:space="preserve">Zócalo de la tragedia</t>
   </si>
   <si>
-    <t xml:space="preserve">01-01-1983</t>
+    <t xml:space="preserve">1983-01-01</t>
   </si>
   <si>
     <t xml:space="preserve">100x70 cm</t>
@@ -89,10 +89,10 @@
     <t xml:space="preserve">obra_id</t>
   </si>
   <si>
-    <t xml:space="preserve">Doble suicidio en "El Sisga"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29-06-1965</t>
+    <t xml:space="preserve">Doble suicidio en El Sisga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1965-06-29</t>
   </si>
   <si>
     <t xml:space="preserve">El Tiempo</t>
@@ -104,13 +104,16 @@
     <t xml:space="preserve">Una indígena y su hijo murieron en persecución</t>
   </si>
   <si>
-    <t xml:space="preserve">24-05-1996</t>
+    <t xml:space="preserve">1996-05-24</t>
   </si>
   <si>
     <t xml:space="preserve">indigena-hijo-el-tiempo.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Láminas de paisajes latinoamericanos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NULL</t>
   </si>
   <si>
     <t xml:space="preserve">laminas-paisajes.jpg</t>
@@ -224,17 +227,17 @@
   </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4453125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.33"/>
   </cols>
   <sheetData>
@@ -336,11 +339,11 @@
   </sheetPr>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4453125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.33"/>
@@ -416,8 +419,14 @@
       <c r="B4" s="0" t="s">
         <v>29</v>
       </c>
+      <c r="C4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>30</v>
+      </c>
       <c r="E4" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>2</v>
@@ -428,10 +437,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>30</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>3</v>

</xml_diff>